<commit_message>
adding gpu train, loss graph
</commit_message>
<xml_diff>
--- a/Results Table.xlsx
+++ b/Results Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Github\Covid-19_Mortality_Rate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE7E046-DFD5-4913-85FD-96A3E54E0175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB7303F7-9B9B-4BFB-A347-4F4BF28CBA97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{D016513F-30A3-42CF-8055-E1036AC92ED9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="16">
   <si>
     <t>Decision Tree</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -84,6 +84,10 @@
   </si>
   <si>
     <t>SVM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CNN</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -5459,10 +5463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41DE40CA-8F40-4AF2-8B4F-98FA1A2B1552}">
-  <dimension ref="A5:I65"/>
+  <dimension ref="A5:I84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="S30" sqref="S30"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C78" sqref="C78:I84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6033,7 +6037,7 @@
         <v>0.91975999999999991</v>
       </c>
     </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
         <v>7</v>
       </c>
@@ -6056,6 +6060,59 @@
         <f t="shared" si="2"/>
         <v>0.76301999999999992</v>
       </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C77" t="s">
+        <v>1</v>
+      </c>
+      <c r="D77" t="s">
+        <v>4</v>
+      </c>
+      <c r="E77" t="s">
+        <v>2</v>
+      </c>
+      <c r="F77" t="s">
+        <v>3</v>
+      </c>
+      <c r="G77" t="s">
+        <v>6</v>
+      </c>
+      <c r="I77" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B78" t="s">
+        <v>8</v>
+      </c>
+      <c r="G78" s="2"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B79" t="s">
+        <v>9</v>
+      </c>
+      <c r="G79" s="2"/>
+    </row>
+    <row r="81" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B81" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="82" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B82" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="84" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B84" t="s">
+        <v>7</v>
+      </c>
+      <c r="G84" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
add hyperparamter trainig, test on loss graph, model checkpoint
</commit_message>
<xml_diff>
--- a/Results Table.xlsx
+++ b/Results Table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Github\Covid-19_Mortality_Rate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB7303F7-9B9B-4BFB-A347-4F4BF28CBA97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCC47E07-63D8-430F-AB19-52ACB08BDF91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{D016513F-30A3-42CF-8055-E1036AC92ED9}"/>
   </bookViews>
@@ -5465,7 +5465,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41DE40CA-8F40-4AF2-8B4F-98FA1A2B1552}">
   <dimension ref="A5:I84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
       <selection activeCell="C78" sqref="C78:I84"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
finish the Federated Learing
</commit_message>
<xml_diff>
--- a/Results Table.xlsx
+++ b/Results Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Github\Covid-19_Mortality_Rate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{930A9860-7133-4A6F-B05A-F716FE3A6972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84DF62E0-6FEA-4CEB-AFE3-2C33DDEAF916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{D016513F-30A3-42CF-8055-E1036AC92ED9}"/>
   </bookViews>
@@ -11763,8 +11763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41DE40CA-8F40-4AF2-8B4F-98FA1A2B1552}">
   <dimension ref="A5:I142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="AE149" sqref="AE149"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>